<commit_message>
chane in static files value
</commit_message>
<xml_diff>
--- a/docs-compose/overwatch_docs/static/assets/DeployOverwatch/080x_overwatch_deployment_config_template.xlsx
+++ b/docs-compose/overwatch_docs/static/assets/DeployOverwatch/080x_overwatch_deployment_config_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aman.Jain/Documents/Overwatch/overwatch/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aman.Jain/Documents/Overwatch/overwatch/docs-compose/overwatch_docs/static/assets/DeployOverwatch/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9AC83C-BF7E-1C4B-93DB-7B8A77E32E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470FD192-9D4F-A840-906F-57CCA12C18E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2760" windowWidth="35840" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>workspace_name</t>
   </si>
@@ -193,9 +193,6 @@
     <t>overwatch_consumer_mws3</t>
   </si>
   <si>
-    <t>aws_audit_log</t>
-  </si>
-  <si>
     <t>example-gcp</t>
   </si>
   <si>
@@ -232,13 +229,10 @@
     <t>sql_endpoint</t>
   </si>
   <si>
-    <t>/sql/1.0/warehouses/123abc456efg</t>
-  </si>
-  <si>
     <t>/sql/1.0/warehouses/789iqa345wer</t>
   </si>
   <si>
-    <t>/sql/1.0/warehouses/567opa125ajk</t>
+    <t>system</t>
   </si>
 </sst>
 </file>
@@ -556,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -689,10 +683,10 @@
         <v>30</v>
       </c>
       <c r="AF1" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG1" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -756,9 +750,7 @@
       <c r="U2" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="AG2" s="7" t="s">
-        <v>72</v>
-      </c>
+      <c r="AG2" s="7"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -822,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="AG3" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.2">
@@ -859,8 +851,8 @@
       <c r="K4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>57</v>
+      <c r="L4" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="O4" s="4">
         <v>0.55000000000000004</v>
@@ -883,31 +875,31 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>59</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" t="s">
-        <v>60</v>
       </c>
       <c r="F5" s="6">
         <v>44701</v>
       </c>
       <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" t="s">
         <v>61</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>62</v>
-      </c>
-      <c r="I5" t="s">
-        <v>63</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>38</v>
@@ -916,7 +908,7 @@
         <v>47</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O5">
         <v>0.55000000000000004</v>
@@ -937,10 +929,7 @@
         <v>1</v>
       </c>
       <c r="AF5" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.2">

</xml_diff>